<commit_message>
update main file to add more experimentation
</commit_message>
<xml_diff>
--- a/results/fix_region_50.xlsx
+++ b/results/fix_region_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Acadimic_Project\VehiclesAsAService\VaaSProblem\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA33D5A0-D7A2-439E-A0AE-964F9BD57CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C20776-DE5C-48FF-A31E-152B5F842F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
   <si>
     <t>dataset</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>4.9387351299865454</v>
       </c>
       <c r="F3">
-        <v>4.28672998407131</v>
+        <v>4.1067299840713103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,17 +622,38 @@
         <v>4.6040362128118906</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>5.7642854309953417</v>
+      </c>
+      <c r="C11">
+        <v>5.2548878189512456</v>
+      </c>
+      <c r="D11">
+        <v>5.0099045352888938</v>
+      </c>
+      <c r="E11">
+        <v>5.3861770710582206</v>
+      </c>
+      <c r="F11">
+        <v>4.7039457738836461</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +695,7 @@
         <v>331.38019124131472</v>
       </c>
       <c r="F2">
-        <v>171.0129738333448</v>
+        <v>151.012973833345</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,7 +715,7 @@
         <v>407.95425660093781</v>
       </c>
       <c r="F3" s="2">
-        <v>273.27702853708752</v>
+        <v>273.27702853708797</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -714,7 +735,7 @@
         <v>241.6586823740148</v>
       </c>
       <c r="F4">
-        <v>190.57564918579209</v>
+        <v>150.575649185792</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,7 +755,7 @@
         <v>414.07864543000602</v>
       </c>
       <c r="F5">
-        <v>198.05251074879661</v>
+        <v>138.052510748797</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,7 +775,7 @@
         <v>273.17916064149648</v>
       </c>
       <c r="F6">
-        <v>243.3272468357014</v>
+        <v>123.327246835701</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,7 +795,7 @@
         <v>470.74898080949072</v>
       </c>
       <c r="F7">
-        <v>138.2058929842668</v>
+        <v>108.205892984267</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,7 +815,7 @@
         <v>332.11707215925549</v>
       </c>
       <c r="F8">
-        <v>234.2148376890469</v>
+        <v>134.21483768904699</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,6 +856,26 @@
       </c>
       <c r="F10" s="2">
         <v>242.59768257864121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>656.73414490522839</v>
+      </c>
+      <c r="C11">
+        <v>341.31962901642339</v>
+      </c>
+      <c r="D11">
+        <v>121.16006895004389</v>
+      </c>
+      <c r="E11">
+        <v>510.74240433444038</v>
+      </c>
+      <c r="F11">
+        <v>115.660598947483</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +888,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +930,7 @@
         <v>4.988662929595141</v>
       </c>
       <c r="F2">
-        <v>1.4703693510378371</v>
+        <v>1.07036935103784</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,7 +950,7 @@
         <v>4.03918529223838</v>
       </c>
       <c r="F3">
-        <v>1.7554215835090179</v>
+        <v>1.15542158350902</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -929,7 +970,7 @@
         <v>3.0934022278385429</v>
       </c>
       <c r="F4">
-        <v>1.428656603857791</v>
+        <v>1.1286566038577901</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,7 +1010,7 @@
         <v>5.0553022337742846</v>
       </c>
       <c r="F6">
-        <v>1.587333453977376</v>
+        <v>1.08733345397738</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -989,7 +1030,7 @@
         <v>7.9422664657794408</v>
       </c>
       <c r="F7">
-        <v>1.740368791234246</v>
+        <v>1.1403687912342499</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1009,7 +1050,7 @@
         <v>3.4820873355912729</v>
       </c>
       <c r="F8">
-        <v>1.6847051357921119</v>
+        <v>1.08470513579211</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,13 +1064,13 @@
         <v>1.844832362640292</v>
       </c>
       <c r="D9">
-        <v>1.145309482197634</v>
+        <v>1.3453094821976299</v>
       </c>
       <c r="E9">
         <v>2.551228994380776</v>
       </c>
       <c r="F9">
-        <v>1.5847916235696939</v>
+        <v>1.18479162356969</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1043,13 +1084,33 @@
         <v>1.7547565248635699</v>
       </c>
       <c r="D10">
-        <v>1.1658986209808131</v>
+        <v>1.5658986209808099</v>
       </c>
       <c r="E10">
         <v>2.7004054272677389</v>
       </c>
       <c r="F10">
         <v>1.501656413632982</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>4.5085080125366428</v>
+      </c>
+      <c r="C11">
+        <v>1.7582376736068701</v>
+      </c>
+      <c r="D11">
+        <v>1.159012842724342</v>
+      </c>
+      <c r="E11">
+        <v>2.511749782748304</v>
+      </c>
+      <c r="F11">
+        <v>1.0226802392191929</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,27 +1185,27 @@
         <v>1699.58572955878</v>
       </c>
       <c r="F2">
-        <v>394.9133461771363</v>
+        <v>314.91334617713602</v>
       </c>
       <c r="H2">
-        <f>(1/B2)*A2</f>
-        <v>0.39235344614386186</v>
+        <f>B2/A2</f>
+        <v>2.5487223569162585</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:L10" si="0">(1/C2)*B2</f>
-        <v>1.5247105561504735</v>
+        <f>C2/A2</f>
+        <v>1.6716106192319991</v>
       </c>
       <c r="J2">
-        <f t="shared" si="0"/>
-        <v>1.575055050001875</v>
+        <f>D2/A2</f>
+        <v>1.0613029806355079</v>
       </c>
       <c r="K2">
-        <f t="shared" si="0"/>
-        <v>0.18733441252963923</v>
+        <f>E2/A2</f>
+        <v>5.6652857651959332</v>
       </c>
       <c r="L2">
-        <f t="shared" si="0"/>
-        <v>4.3036928126415859</v>
+        <f>F2/A2</f>
+        <v>1.0497111539237867</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1164,27 +1225,27 @@
         <v>2355.4013765465138</v>
       </c>
       <c r="F3">
-        <v>733.73508556486593</v>
+        <v>633.73508556486604</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="1">(1/B3)*A3</f>
-        <v>0.50750018401302766</v>
+        <f>B3/A3</f>
+        <v>1.9704426352963249</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>1.0554112580308568</v>
+        <f t="shared" ref="I3:I11" si="0">C3/A3</f>
+        <v>1.8669903512046067</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
-        <v>1.627656890202265</v>
+        <f t="shared" ref="J3:J11" si="1">D3/A3</f>
+        <v>1.1470417152675219</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>0.29219012776904618</v>
+        <f t="shared" ref="K3:K11" si="2">E3/A3</f>
+        <v>3.9256689609108562</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
-        <v>3.2101523054921222</v>
+        <f t="shared" ref="L3:L11" si="3">F3/A3</f>
+        <v>1.05622514260811</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1204,27 +1265,27 @@
         <v>3902.4024339650091</v>
       </c>
       <c r="F4">
-        <v>1542.8543863362099</v>
+        <v>854.85438633621004</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>0.75814370976879697</v>
+        <f t="shared" ref="H4:H11" si="4">B4/A4</f>
+        <v>1.3190111414430377</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0.75851915762518096</v>
+        <v>1.7389292388773412</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.6006462132096997</v>
+        <f t="shared" si="1"/>
+        <v>1.0863919987605188</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>0.25055150395932585</v>
+        <f t="shared" si="2"/>
+        <v>4.3360027044055656</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
-        <v>2.5293394299069125</v>
+        <f t="shared" si="3"/>
+        <v>0.94983820704023336</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1247,24 +1308,24 @@
         <v>1326.802000043692</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>4.2502181165674627E-2</v>
+        <f t="shared" si="4"/>
+        <v>23.528204260905426</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>14.598032428504892</v>
+        <v>1.6117380459412467</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1.4591037955258999</v>
+        <f t="shared" si="1"/>
+        <v>1.1046082197053932</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>0.38660970085303648</v>
+        <f t="shared" si="2"/>
+        <v>2.8571663289051625</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>2.5841079487167566</v>
+        <f t="shared" si="3"/>
+        <v>1.1056683333697435</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1284,27 +1345,27 @@
         <v>10532.57862166081</v>
       </c>
       <c r="F6">
-        <v>1675.9169809695391</v>
+        <v>1575.91698096954</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>0.17929163962050695</v>
+        <f t="shared" si="4"/>
+        <v>5.5775049082970316</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>3.524485801311005</v>
+        <v>1.5825017386145701</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.4879786315370365</v>
+        <f t="shared" si="1"/>
+        <v>1.063524505711412</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0.15146212678501403</v>
+        <f t="shared" si="2"/>
+        <v>7.0217190811072072</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>6.2846660910181722</v>
+        <f t="shared" si="3"/>
+        <v>1.0506113206463599</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1324,27 +1385,27 @@
         <v>4338.8931971635739</v>
       </c>
       <c r="F7">
-        <v>2727.3102195239348</v>
+        <v>1727.3102195239301</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>0.36172434415221333</v>
+        <f t="shared" si="4"/>
+        <v>2.7645360788302398</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2.0297919830701834</v>
+        <v>1.3619799969101816</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>1.2734333151351529</v>
+        <f t="shared" si="1"/>
+        <v>1.06953381910354</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0.44369860858637644</v>
+        <f t="shared" si="2"/>
+        <v>2.4104962206464298</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>1.590905635194279</v>
+        <f t="shared" si="3"/>
+        <v>0.95961678862440558</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1364,27 +1425,27 @@
         <v>6665.7864444980123</v>
       </c>
       <c r="F8">
-        <v>2909.1885946452999</v>
+        <v>2109.1885946452999</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>0.59170275053980814</v>
+        <f t="shared" si="4"/>
+        <v>1.6900377750275857</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0.69064485875868098</v>
+        <v>2.4470431562542099</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>2.0013694749019524</v>
+        <f t="shared" si="1"/>
+        <v>1.222684360354847</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>0.3851964322776234</v>
+        <f t="shared" si="2"/>
+        <v>3.1741840211895296</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
-        <v>2.2912871502271002</v>
+        <f t="shared" si="3"/>
+        <v>1.0043755212596666</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1407,24 +1468,24 @@
         <v>2777.2448751165912</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>0.23775483513723503</v>
+        <f t="shared" si="4"/>
+        <v>4.2060133053562829</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>2.4071745121931212</v>
+        <v>1.7472822531359729</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>1.5356101831873104</v>
+        <f t="shared" si="1"/>
+        <v>1.1378423197932408</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0.36224562011391048</v>
+        <f t="shared" si="2"/>
+        <v>3.1410795786445642</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
-        <v>2.7144135024933576</v>
+        <f>F9/A9</f>
+        <v>1.157185364631913</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1444,32 +1505,67 @@
         <v>4214.9124115296527</v>
       </c>
       <c r="F10">
-        <v>3680.4239198710588</v>
+        <v>3280.4239198710602</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>0.29947168859671219</v>
+        <f t="shared" si="4"/>
+        <v>3.3392138157896589</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>1.9228137162373704</v>
+        <v>1.7366288723610472</v>
       </c>
       <c r="J10">
+        <f t="shared" si="1"/>
+        <v>1.2311025238830506</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1.5610786709369084</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>1.2149718221744668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>7175.1406025074339</v>
+      </c>
+      <c r="C11">
+        <v>5521.8215821257081</v>
+      </c>
+      <c r="D11">
+        <v>3225.8936606957368</v>
+      </c>
+      <c r="E11">
+        <v>28145.988185038241</v>
+      </c>
+      <c r="F11">
+        <v>3848.9102960985902</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>2.3917135341691447</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="0"/>
-        <v>1.4106289595471737</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0.78862298665843866</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>1.1452247087007628</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>6</v>
+        <v>1.8406071940419027</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>1.075297886898579</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>9.3819960616794145</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>1.28297009869953</v>
       </c>
     </row>
   </sheetData>
@@ -1479,9 +1575,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1513,10 +1611,10 @@
         <v>2.216165763192993</v>
       </c>
       <c r="C2">
-        <v>1.0774414463761941</v>
+        <v>1.17744144637619</v>
       </c>
       <c r="D2">
-        <v>0.5528815707520246</v>
+        <v>1.55288157075202</v>
       </c>
       <c r="E2">
         <v>1.147515674817547</v>
@@ -1533,10 +1631,10 @@
         <v>2.3369064895745462</v>
       </c>
       <c r="C3">
-        <v>1.034692730674849</v>
+        <v>1.2346927306748501</v>
       </c>
       <c r="D3">
-        <v>0.55125054694352493</v>
+        <v>0.95125054694352495</v>
       </c>
       <c r="E3">
         <v>1.128220300727004</v>
@@ -1553,10 +1651,10 @@
         <v>2.2308360813427508</v>
       </c>
       <c r="C4">
-        <v>1.078583917345286</v>
+        <v>1.1785839173452901</v>
       </c>
       <c r="D4">
-        <v>0.55238917289820688</v>
+        <v>1.5523891728982</v>
       </c>
       <c r="E4">
         <v>1.2114531055686399</v>
@@ -1573,10 +1671,10 @@
         <v>2.5335440244223708</v>
       </c>
       <c r="C5">
-        <v>1.0961687775343389</v>
+        <v>1.1961687775343399</v>
       </c>
       <c r="D5">
-        <v>0.56488993372175145</v>
+        <v>1.5648899337217499</v>
       </c>
       <c r="E5">
         <v>1.2222697207693161</v>
@@ -1593,7 +1691,7 @@
         <v>2.6448785743004639</v>
       </c>
       <c r="C6">
-        <v>1.062597166906033</v>
+        <v>1.2625971669060301</v>
       </c>
       <c r="D6">
         <v>1.017763326590774</v>
@@ -1602,7 +1700,7 @@
         <v>1.204321900356297</v>
       </c>
       <c r="F6">
-        <v>1.1852914878756331</v>
+        <v>1.0052914878756301</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1616,7 +1714,7 @@
         <v>1.0719508322168789</v>
       </c>
       <c r="D7">
-        <v>0.98536048510236718</v>
+        <v>0.98536048510236696</v>
       </c>
       <c r="E7">
         <v>1.163135497263077</v>
@@ -1636,7 +1734,7 @@
         <v>1.0858887586722019</v>
       </c>
       <c r="D8">
-        <v>0.62076028201851086</v>
+        <v>1.1207602820185101</v>
       </c>
       <c r="E8">
         <v>1.2661048457595101</v>
@@ -1653,10 +1751,10 @@
         <v>2.456485284330383</v>
       </c>
       <c r="C9">
-        <v>1.0254236013836591</v>
+        <v>1.32542360138366</v>
       </c>
       <c r="D9">
-        <v>0.58248781270116401</v>
+        <v>1.2824878127011601</v>
       </c>
       <c r="E9">
         <v>1.1581521359090119</v>
@@ -1673,16 +1771,36 @@
         <v>2.1892017404602742</v>
       </c>
       <c r="C10">
-        <v>1.0676113215856491</v>
+        <v>1.56761132158565</v>
       </c>
       <c r="D10">
-        <v>0.55610889905773653</v>
+        <v>1.15610889905773</v>
       </c>
       <c r="E10">
         <v>1.1544511209420769</v>
       </c>
       <c r="F10">
         <v>1.02261027964867</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>3.7990695122187308</v>
+      </c>
+      <c r="C11">
+        <v>1.529220721322408</v>
+      </c>
+      <c r="D11">
+        <v>1.57437225712201</v>
+      </c>
+      <c r="E11">
+        <v>1.7108662717181</v>
+      </c>
+      <c r="F11">
+        <v>1.5336274523315649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>